<commit_message>
toggle LED by touch_button
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="47">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -141,6 +141,21 @@
   </si>
   <si>
     <t xml:space="preserve">Small</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LTR</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Toggle LED</t>
   </si>
 </sst>
 </file>
@@ -1601,6 +1616,23 @@
         <v>36</v>
       </c>
     </row>
+    <row r="4">
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
show dynamic msg to UI
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="53">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -156,6 +156,24 @@
   </si>
   <si>
     <t xml:space="preserve">Toggle LED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x20-0x7E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Left</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RX: &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">default</t>
   </si>
 </sst>
 </file>
@@ -1399,7 +1417,9 @@
       </c>
       <c r="G4"/>
       <c r="H4"/>
-      <c r="I4"/>
+      <c r="I4" t="s">
+        <v>47</v>
+      </c>
       <c r="J4"/>
       <c r="L4" s="4" t="s">
         <v>9</v>
@@ -1633,6 +1653,40 @@
         <v>46</v>
       </c>
     </row>
+    <row r="5">
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
can send pulse with data
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="61">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1431,7 +1431,7 @@
         <v>39</v>
       </c>
       <c r="D4">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E4">
         <v>4</v>

</xml_diff>